<commit_message>
1.create package 2.create user manager sql script 3.add user manager outline designe
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,10 +214,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户ID，使用UUID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -230,10 +226,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户密码，使用MD5(base64)加密</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -246,10 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户角色</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -258,11 +246,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>微信用户对公众号的唯一ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户角色表——role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>roleid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>微信用户对公众号的唯一ID</t>
+    <t>角色ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色类型，包含艺人，买家，系统管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户所在的分组ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户的标识，对当前公众号唯一</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -270,195 +306,210 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户角色表——role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户表——userInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字段名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>roleid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色类型，包含艺人，买家，系统管理员</t>
+    <t>通过微信客户端注册的用户，在用户表和微信用户表中同时有纪录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nickname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信用户的昵称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户的性别，值为1时是男性，值为2时是女性，值为0时是未知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户所在城市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>country</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户所在国家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户所在省份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>language</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户的语言，简体中文为zh_CN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户头像，最后一个数值代表正方形头像大小（有0、46、64、96、132数值可选，0代表640*640正方形头像），用户没有头像时该项为空。若用户更换头像，原有头像URL将失效。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户关注时间，为时间戳。如果用户曾多次关注，则取最后关注时间"subscribe_time": 1382694957</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只有在用户将公众号绑定到微信开放平台帐号后，才会出现该字段。详见：获取用户个人信息（UnionID机制）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公众号运营者对粉丝的备注，公众号运营者可在微信公众平台用户管理界面对粉丝添加备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户表——user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信用户信息表－user_wechat_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rolename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifydate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一次修改时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastlogindate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一次登陆时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rolename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roledesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createuserid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建的用户ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifyuserid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一次修改的用户ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modifydate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一次修改时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>province</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>headimgurl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subscribe_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unionid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remark</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户所在的分组ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>openid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户的标识，对当前公众号唯一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过微信客户端注册的用户，在用户表和微信用户表中同时有纪录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nickname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(64)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>微信用户的昵称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>char(1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户的性别，值为1时是男性，值为2时是女性，值为0时是未知</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户所在城市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>country</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户所在国家</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>province</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户所在省份</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>language</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户的语言，简体中文为zh_CN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>headimgurl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户头像，最后一个数值代表正方形头像大小（有0、46、64、96、132数值可选，0代表640*640正方形头像），用户没有头像时该项为空。若用户更换头像，原有头像URL将失效。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>subscribe_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户关注时间，为时间戳。如果用户曾多次关注，则取最后关注时间"subscribe_time": 1382694957</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unionid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>只有在用户将公众号绑定到微信开放平台帐号后，才会出现该字段。详见：获取用户个人信息（UnionID机制）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>公众号运营者对粉丝的备注，公众号运营者可在微信公众平台用户管理界面对粉丝添加备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>微信用户信息表－user_wechat_info</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -645,8 +696,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,6 +729,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -680,12 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -701,19 +762,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="23">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1056,12 +1127,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -1078,7 +1149,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1088,7 +1159,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1169,7 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1106,7 +1177,7 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1185,7 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1193,7 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="7"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1204,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="7"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1141,7 +1212,7 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="7"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1149,7 +1220,7 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1157,13 +1228,13 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1173,7 +1244,7 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1254,7 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1262,7 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="7"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1199,7 +1270,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1207,7 +1278,7 @@
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1215,7 +1286,7 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1225,7 +1296,7 @@
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1235,7 +1306,7 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1243,7 +1314,7 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1251,7 +1322,7 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1330,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="8"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1267,7 +1338,7 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1277,7 +1348,7 @@
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="7"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1287,7 +1358,7 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="7"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
@@ -1295,7 +1366,7 @@
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="7"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1303,7 +1374,7 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="7"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1311,7 +1382,7 @@
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="8"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1379,16 +1450,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="158.5" bestFit="1" customWidth="1"/>
@@ -1411,358 +1482,470 @@
       <c r="L1" s="13"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="7">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="6">
+        <v>7</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="7">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="6">
+        <v>8</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="6">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="6">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="F16" s="6">
+        <v>11</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="F17" s="6">
+        <v>12</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="F18" s="6">
+        <v>13</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="7">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="10" t="s">
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="7">
+        <v>3</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="7">
+        <v>4</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="7">
+        <v>5</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="12">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="11">
-        <v>1</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="12">
-        <v>2</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="11">
-        <v>2</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="12">
-        <v>3</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="11">
-        <v>3</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="12">
-        <v>4</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="11">
-        <v>4</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="12">
-        <v>5</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="11">
-        <v>5</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="12">
+      <c r="D24" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="11">
-        <v>6</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="12">
+      <c r="B25" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="11">
-        <v>7</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="F13" s="11">
-        <v>8</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="F14" s="11">
-        <v>9</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="F15" s="11">
-        <v>10</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="11">
-        <v>11</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="12">
-        <v>1</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="11">
-        <v>12</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="12">
-        <v>2</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="11">
-        <v>13</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>74</v>
+      <c r="B26" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A18:D18"/>
     <mergeCell ref="F4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add order table design and dao entities
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="开发计划时间安排" sheetId="1" r:id="rId1"/>
-    <sheet name="表结构设计" sheetId="2" r:id="rId2"/>
+    <sheet name="表结构设计-user" sheetId="2" r:id="rId2"/>
+    <sheet name="表结构设计－order" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="161">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -510,6 +511,158 @@
   </si>
   <si>
     <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出时间，不可为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户订单表－order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>orderid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单ID，主键，使用UUID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linkman_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系人姓名，默认是下单人的姓名，但是可以需改，不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系电话，默认是下单人的手机号，不可为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(128)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show_fee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预计演出金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request_mark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出需求，由用户填写，需要什么类型的节目，看中哪些艺人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下单人用户ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信公众号关注用户的id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show_addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modify_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单修改时间，客户代表谈完后修改金额之类的事宜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定单创建时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单修改人ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modify_userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,7 +849,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -720,8 +873,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -761,8 +934,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="43">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -774,6 +953,16 @@
     <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -785,6 +974,16 @@
     <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1452,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1496,28 +1695,28 @@
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1534,7 +1733,7 @@
       <c r="D6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="17">
         <v>1</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -1560,7 +1759,7 @@
       <c r="D7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="17">
         <v>2</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -1586,7 +1785,7 @@
       <c r="D8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="17">
         <v>3</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1612,7 +1811,7 @@
       <c r="D9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="17">
         <v>4</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -1638,7 +1837,7 @@
       <c r="D10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="17">
         <v>5</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -1664,7 +1863,7 @@
       <c r="D11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="17">
         <v>6</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -1690,7 +1889,7 @@
       <c r="D12" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="17">
         <v>7</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1716,7 +1915,7 @@
       <c r="D13" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="17">
         <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -1742,7 +1941,7 @@
       <c r="D14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="17">
         <v>9</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -1768,7 +1967,7 @@
       <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="17">
         <v>10</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -1782,7 +1981,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="F16" s="6">
+      <c r="F16" s="17">
         <v>11</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -1796,7 +1995,7 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="F17" s="6">
+      <c r="F17" s="17">
         <v>12</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -1816,7 +2015,7 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
-      <c r="F18" s="6">
+      <c r="F18" s="17">
         <v>13</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1830,16 +2029,16 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1957,4 +2156,223 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7">
+        <v>11</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add actor table desinge
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\git\showmecoo\showmecoo-web-docs\src\main\resources\设计文档\概要设计\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="25515" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="开发计划时间安排" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="212">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -667,11 +672,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>艺人年龄，如果是团体可不填，或填团队成立时间，非必填项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>舞蹈演员表－actor_dancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>艺人表－actor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar（45）</t>
+    <t>actor表用于艺人一级页面的展示,以及点击更多的时候用于展示的表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -679,7 +696,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>actorid</t>
+    <t>用于演员二级页面艺人详情展示以及简介，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擅长舞种，以逗号分割的字符串，eg 街舞，机械舞，爵士舞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代表演出，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主形象照名，大图，上传到服务器后的名字，用于默认的大图展示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介，艺人自我简短介绍，不超过140个字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身高,厘米为单位，如果是模特和主持人，则必填，否则为非必填项，此项由前段页面控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出费用，不明确标出，作为以后的预留字段，如果为0则在页面写上“面议（总有惊喜）”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skilled_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>payment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>standard_display</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(512)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mian_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(256)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief_intro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(32)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -687,43 +796,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar（32）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>varchar(45)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人年龄，如果是团体可不填，或填团队成立时间，非必填项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>身高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人类型：舞者，歌手，模特，主持人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>如果是模特和主持人，则必填，否则为非必填项，此项由前段页面控制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出演次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>粉丝数</t>
+    <t>才艺风格，一级页面中每种风格的艺人只展示部分，点击更多查看全部。舞蹈分为街舞，流行舞，歌手分为摇滚，流行等，模特分为男模，女模；主持人分为男主持，女主持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displayed_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出演次数,参与过演出的次数，初始值按照艺人等级划分，公司将艺人分为高中低三个层级，初次录入资料的时候根据层级以及具体情况给定演出次数，以后每演出一次加一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visit_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被查看次数，艺人被查看的次数，用户不需要登陆，只要点击了该艺人进入二级页面，查看次数+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fans_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粉丝数，爱心符号的标识，只有会员才可以点，点爱心标志，粉丝数+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -731,11 +868,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>舞蹈演员表－dancer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人ID</t>
+    <t>imageName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>形象照名，照片上传到服务器后的名字，存放形象照的目录固定，</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1021,58 +1158,66 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1404,13 +1549,13 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +1563,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1432,7 +1577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
@@ -1442,7 +1587,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -1452,7 +1597,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1460,7 +1605,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1468,7 +1613,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1476,7 +1621,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1487,7 +1632,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -1495,7 +1640,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
         <v>11</v>
@@ -1503,7 +1648,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="12"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1511,13 +1656,13 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
@@ -1527,7 +1672,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
         <v>18</v>
@@ -1537,7 +1682,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
@@ -1545,7 +1690,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -1553,7 +1698,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
         <v>16</v>
@@ -1561,7 +1706,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1569,7 +1714,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -1579,7 +1724,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -1589,7 +1734,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="12"/>
       <c r="B21" s="2" t="s">
         <v>23</v>
@@ -1597,7 +1742,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="12"/>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -1605,7 +1750,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="12"/>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -1613,7 +1758,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>26</v>
@@ -1621,7 +1766,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="11" t="s">
         <v>27</v>
       </c>
@@ -1631,7 +1776,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
         <v>28</v>
@@ -1641,7 +1786,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="12"/>
       <c r="B27" s="2" t="s">
         <v>29</v>
@@ -1649,7 +1794,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12"/>
       <c r="B28" s="2" t="s">
         <v>30</v>
@@ -1657,7 +1802,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="12"/>
       <c r="B29" s="2" t="s">
         <v>31</v>
@@ -1665,7 +1810,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="13"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
@@ -1673,7 +1818,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -1683,7 +1828,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1693,7 +1838,7 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -1703,7 +1848,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -1723,7 +1868,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPUBLIC</oddFooter>
+    <evenFooter>&amp;LPUBLIC</evenFooter>
+    <firstFooter>&amp;LPUBLIC</firstFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1736,11 +1886,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F29" sqref="F29:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -1749,7 +1899,7 @@
     <col min="9" max="9" width="158.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25">
+    <row r="1" spans="1:12" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -1765,7 +1915,7 @@
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>88</v>
       </c>
@@ -1779,7 +1929,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>47</v>
       </c>
@@ -1805,7 +1955,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -1831,7 +1981,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -1857,7 +2007,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -1883,7 +2033,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>4</v>
       </c>
@@ -1909,7 +2059,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>5</v>
       </c>
@@ -1935,7 +2085,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>6</v>
       </c>
@@ -1961,7 +2111,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>7</v>
       </c>
@@ -1987,7 +2137,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>8</v>
       </c>
@@ -2013,7 +2163,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>9</v>
       </c>
@@ -2039,7 +2189,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>10</v>
       </c>
@@ -2065,7 +2215,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="F16" s="8">
         <v>11</v>
       </c>
@@ -2079,7 +2229,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="F17" s="8">
         <v>12</v>
       </c>
@@ -2093,7 +2243,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>61</v>
       </c>
@@ -2113,7 +2263,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>62</v>
       </c>
@@ -2127,7 +2277,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -2141,7 +2291,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="7">
         <v>2</v>
       </c>
@@ -2155,7 +2305,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="7">
         <v>3</v>
       </c>
@@ -2169,7 +2319,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="7">
         <v>4</v>
       </c>
@@ -2183,7 +2333,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="7">
         <v>5</v>
       </c>
@@ -2197,7 +2347,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="7">
         <v>6</v>
       </c>
@@ -2211,7 +2361,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="7">
         <v>7</v>
       </c>
@@ -2234,7 +2384,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPUBLIC</oddFooter>
+    <evenFooter>&amp;LPUBLIC</evenFooter>
+    <firstFooter>&amp;LPUBLIC</firstFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2248,16 +2403,16 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>127</v>
       </c>
@@ -2265,7 +2420,7 @@
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>123</v>
       </c>
@@ -2279,7 +2434,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -2293,7 +2448,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -2307,7 +2462,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -2321,7 +2476,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -2335,7 +2490,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -2349,7 +2504,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -2363,7 +2518,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -2377,7 +2532,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -2391,7 +2546,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -2405,7 +2560,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -2419,7 +2574,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -2433,7 +2588,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -2453,7 +2608,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPUBLIC</oddFooter>
+    <evenFooter>&amp;LPUBLIC</evenFooter>
+    <firstFooter>&amp;LPUBLIC</firstFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2464,20 +2624,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E19"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="169.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
@@ -2491,75 +2664,146 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>6</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>167</v>
       </c>
-      <c r="C6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="16" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="D8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="D10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="D11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="D12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="D13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
@@ -2573,15 +2817,173 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="D19" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="7">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="7">
+        <v>3</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>178</v>
       </c>
+      <c r="C21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="7">
+        <v>4</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="7">
+        <v>5</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="7">
+        <v>6</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="7">
+        <v>7</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="7">
+        <v>8</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="7">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="7">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="7">
+        <v>11</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPUBLIC</oddFooter>
+    <evenFooter>&amp;LPUBLIC</evenFooter>
+    <firstFooter>&amp;LPUBLIC</firstFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add actor module 表结构设计
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\git\showmecoo\showmecoo-web-docs\src\main\resources\设计文档\概要设计\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="25515" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="开发计划时间安排" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="233">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -704,111 +699,239 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>代表演出，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主形象照名，大图，上传到服务器后的名字，用于默认的大图展示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介，艺人自我简短介绍，不超过140个字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身高,厘米为单位，如果是模特和主持人，则必填，否则为非必填项，此项由前段页面控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出费用，不明确标出，作为以后的预留字段，如果为0则在页面写上“面议（总有惊喜）”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skilled_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(512)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mian_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(256)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar（32）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>才艺风格，一级页面中每种风格的艺人只展示部分，点击更多查看全部。舞蹈分为街舞，流行舞，歌手分为摇滚，流行等，模特分为男模，女模；主持人分为男主持，女主持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displayed_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出演次数,参与过演出的次数，初始值按照艺人等级划分，公司将艺人分为高中低三个层级，初次录入资料的时候根据层级以及具体情况给定演出次数，以后每演出一次加一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visit_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被查看次数，艺人被查看的次数，用户不需要登陆，只要点击了该艺人进入二级页面，查看次数+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fans_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粉丝数，爱心符号的标识，只有会员才可以点，点爱心标志，粉丝数+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入时间，加入showmecoo公司的时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imageName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>形象照名，照片上传到服务器后的名字，存放形象照的目录固定，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人等级评分，80－100的为高级，40-79的为中级，0-39的为低级，前期评分为主观评定，录入艺人的时候给打的分数，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level_score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>代表演出，以逗号分割的字符串</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主形象照名，大图，上传到服务器后的名字，用于默认的大图展示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>简介，艺人自我简短介绍，不超过140个字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>actorId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>身高,厘米为单位，如果是模特和主持人，则必填，否则为非必填项，此项由前段页面控制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出费用，不明确标出，作为以后的预留字段，如果为0则在页面写上“面议（总有惊喜）”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>height</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skilled_style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_addr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>payment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>standard_display</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(512)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mian_image_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>second_image_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(256)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>brief_intro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>actorId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar（32）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kind</t>
+    <t>代表作品，唱的比较好的曲目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief_introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represantive_work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief_introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level_score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擅长的曲目风格，以逗号分割的字符串，eg：摇滚，流行，民俗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>歌手演员表－actor_singer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模特演员表－actor_model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别，男（1），女（2）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -816,63 +939,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>才艺风格，一级页面中每种风格的艺人只展示部分，点击更多查看全部。舞蹈分为街舞，流行舞，歌手分为摇滚，流行等，模特分为男模，女模；主持人分为男主持，女主持</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>displayed_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出演次数,参与过演出的次数，初始值按照艺人等级划分，公司将艺人分为高中低三个层级，初次录入资料的时候根据层级以及具体情况给定演出次数，以后每演出一次加一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visit_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>被查看次数，艺人被查看的次数，用户不需要登陆，只要点击了该艺人进入二级页面，查看次数+1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fans_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>粉丝数，爱心符号的标识，只有会员才可以点，点爱心标志，粉丝数+1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>加入时间，加入showmecoo公司的时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imageName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>形象照名，照片上传到服务器后的名字，存放形象照的目录固定，</t>
+    <t>sex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模特的一级页面暂时按照男模和女模来区分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主持人演员表－actor_compere</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主持人的一级页面暂时按照男模和女模来区分</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1059,7 +1138,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1108,6 +1187,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
@@ -1157,56 +1264,84 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="77">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1549,13 +1684,13 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="25.5">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1563,7 +1698,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
@@ -1587,7 +1722,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -1597,7 +1732,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1605,7 +1740,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1613,7 +1748,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1621,7 +1756,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1632,7 +1767,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -1640,7 +1775,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
         <v>11</v>
@@ -1648,7 +1783,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="12"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1656,13 +1791,13 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="13"/>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
@@ -1672,7 +1807,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
         <v>18</v>
@@ -1682,7 +1817,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
@@ -1690,7 +1825,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -1698,7 +1833,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
         <v>16</v>
@@ -1706,7 +1841,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1714,7 +1849,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
@@ -1724,7 +1859,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -1734,7 +1869,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21" s="12"/>
       <c r="B21" s="2" t="s">
         <v>23</v>
@@ -1742,7 +1877,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="12"/>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -1750,7 +1885,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="12"/>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -1758,7 +1893,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>26</v>
@@ -1766,7 +1901,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25" s="11" t="s">
         <v>27</v>
       </c>
@@ -1776,7 +1911,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
         <v>28</v>
@@ -1786,7 +1921,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27" s="12"/>
       <c r="B27" s="2" t="s">
         <v>29</v>
@@ -1794,7 +1929,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28" s="12"/>
       <c r="B28" s="2" t="s">
         <v>30</v>
@@ -1802,7 +1937,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29" s="12"/>
       <c r="B29" s="2" t="s">
         <v>31</v>
@@ -1810,7 +1945,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="A30" s="13"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
@@ -1818,7 +1953,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -1828,7 +1963,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1838,7 +1973,7 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -1848,7 +1983,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -1868,7 +2003,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;LPUBLIC</oddFooter>
     <evenFooter>&amp;LPUBLIC</evenFooter>
@@ -1886,11 +2021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -1899,7 +2034,7 @@
     <col min="9" max="9" width="158.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="27">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -1915,7 +2050,7 @@
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12">
       <c r="A4" s="14" t="s">
         <v>88</v>
       </c>
@@ -1929,7 +2064,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12">
       <c r="A5" s="8" t="s">
         <v>47</v>
       </c>
@@ -1955,7 +2090,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -1981,7 +2116,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -2007,7 +2142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -2033,7 +2168,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12">
       <c r="A9" s="7">
         <v>4</v>
       </c>
@@ -2059,7 +2194,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12">
       <c r="A10" s="7">
         <v>5</v>
       </c>
@@ -2085,7 +2220,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12">
       <c r="A11" s="7">
         <v>6</v>
       </c>
@@ -2111,7 +2246,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12">
       <c r="A12" s="7">
         <v>7</v>
       </c>
@@ -2137,7 +2272,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12">
       <c r="A13" s="7">
         <v>8</v>
       </c>
@@ -2163,7 +2298,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12">
       <c r="A14" s="7">
         <v>9</v>
       </c>
@@ -2189,7 +2324,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12">
       <c r="A15" s="7">
         <v>10</v>
       </c>
@@ -2215,7 +2350,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12">
       <c r="F16" s="8">
         <v>11</v>
       </c>
@@ -2229,7 +2364,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="F17" s="8">
         <v>12</v>
       </c>
@@ -2243,7 +2378,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="A18" s="16" t="s">
         <v>61</v>
       </c>
@@ -2263,7 +2398,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" s="8" t="s">
         <v>62</v>
       </c>
@@ -2277,7 +2412,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -2291,7 +2426,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" s="7">
         <v>2</v>
       </c>
@@ -2305,7 +2440,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" s="7">
         <v>3</v>
       </c>
@@ -2319,7 +2454,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="A23" s="7">
         <v>4</v>
       </c>
@@ -2333,7 +2468,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="7">
         <v>5</v>
       </c>
@@ -2347,7 +2482,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="A25" s="7">
         <v>6</v>
       </c>
@@ -2361,7 +2496,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" s="7">
         <v>7</v>
       </c>
@@ -2384,7 +2519,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;LPUBLIC</oddFooter>
     <evenFooter>&amp;LPUBLIC</evenFooter>
@@ -2406,13 +2541,13 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
         <v>127</v>
       </c>
@@ -2420,7 +2555,7 @@
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>123</v>
       </c>
@@ -2434,7 +2569,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -2448,7 +2583,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -2462,7 +2597,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -2476,7 +2611,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -2490,7 +2625,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -2504,7 +2639,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -2518,7 +2653,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -2532,7 +2667,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -2546,7 +2681,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -2560,7 +2695,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -2574,7 +2709,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -2588,7 +2723,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -2608,7 +2743,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;LPUBLIC</oddFooter>
     <evenFooter>&amp;LPUBLIC</evenFooter>
@@ -2624,25 +2759,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D29"/>
+  <dimension ref="A2:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="169.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="169.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" s="16" t="s">
         <v>164</v>
       </c>
@@ -2650,7 +2785,7 @@
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
@@ -2664,321 +2799,852 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="7">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="7">
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="7">
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>196</v>
+        <v>92</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="7">
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>199</v>
+        <v>92</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="7">
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="7">
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="7">
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="7">
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="7">
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7">
+        <v>10</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="7">
+        <v>11</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="7">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="7">
+        <v>2</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="7">
+        <v>5</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7">
+        <v>6</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="7">
-        <v>1</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="7">
-        <v>2</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="7">
-        <v>3</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="9" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="7">
+        <v>7</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="7">
-        <v>4</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="7">
-        <v>5</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="7">
-        <v>6</v>
-      </c>
-      <c r="B24" s="9" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="7">
+        <v>8</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="7">
-        <v>7</v>
-      </c>
-      <c r="B25" s="9" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" s="7">
+        <v>9</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="7">
-        <v>8</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="C28" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="7">
+        <v>10</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="7">
-        <v>9</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="7">
-        <v>10</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="7">
-        <v>11</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>184</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7">
+        <v>11</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="7">
+        <v>12</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="7">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>173</v>
       </c>
+      <c r="C36" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="7">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="7">
+        <v>3</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="7">
+        <v>4</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="7">
+        <v>5</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="7">
+        <v>6</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="7">
+        <v>7</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="7">
+        <v>8</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="7">
+        <v>9</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="7">
+        <v>10</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="7">
+        <v>11</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="18"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="7">
+        <v>1</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="7">
+        <v>2</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="7">
+        <v>3</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="7">
+        <v>4</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="7">
+        <v>5</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="7">
+        <v>7</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="7">
+        <v>8</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="7">
+        <v>9</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="7">
+        <v>10</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="7">
+        <v>11</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="7">
+        <v>1</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="7">
+        <v>2</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="7">
+        <v>3</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="7">
+        <v>4</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="7">
+        <v>5</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="7">
+        <v>7</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="7">
+        <v>8</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="7">
+        <v>9</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="7">
+        <v>10</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="7">
+        <v>11</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A17:D17"/>
+  <mergeCells count="5">
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A65:D65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;LPUBLIC</oddFooter>
     <evenFooter>&amp;LPUBLIC</evenFooter>

</xml_diff>

<commit_message>
add actor serious table repository and bo model
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="239">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -547,10 +547,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>订单ID，主键，使用UUID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -603,10 +599,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>下单人用户ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -687,39 +679,283 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>艺人名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用于演员二级页面艺人详情展示以及简介，</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>代表演出，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主形象照名，大图，上传到服务器后的名字，用于默认的大图展示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介，艺人自我简短介绍，不超过140个字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身高,厘米为单位，如果是模特和主持人，则必填，否则为非必填项，此项由前段页面控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出费用，不明确标出，作为以后的预留字段，如果为0则在页面写上“面议（总有惊喜）”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skilled_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(512)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mian_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(256)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>才艺风格，一级页面中每种风格的艺人只展示部分，点击更多查看全部。舞蹈分为街舞，流行舞，歌手分为摇滚，流行等，模特分为男模，女模；主持人分为男主持，女主持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displayed_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出演次数,参与过演出的次数，初始值按照艺人等级划分，公司将艺人分为高中低三个层级，初次录入资料的时候根据层级以及具体情况给定演出次数，以后每演出一次加一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visit_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被查看次数，艺人被查看的次数，用户不需要登陆，只要点击了该艺人进入二级页面，查看次数+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fans_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粉丝数，爱心符号的标识，只有会员才可以点，点爱心标志，粉丝数+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入时间，加入showmecoo公司的时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>形象照名，照片上传到服务器后的名字，存放形象照的目录固定，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人等级评分，80－100的为高级，40-79的为中级，0-39的为低级，前期评分为主观评定，录入艺人的时候给打的分数，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level_score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief_introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represantive_work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief_introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level_score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>歌手演员表－actor_singer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模特演员表－actor_model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主持人演员表－actor_compere</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar（45）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nick_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别，男（1），女（2）,必填字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人艺名，唯一字段，用于展示艺名以及区分重名艺人，必填字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人名字，必填字段t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>擅长舞种，以逗号分割的字符串，eg 街舞，机械舞，爵士舞</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>艺人等级评分，80－100的为高级，40-79的为中级，0-39的为低级，前期评分为主观评定，录入艺人的时候给打的分数，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介，艺人自我简短介绍，不超过140个字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>代表演出，以逗号分割的字符串</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>主形象照名，大图，上传到服务器后的名字，用于默认的大图展示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>简介，艺人自我简短介绍，不超过140个字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>actorId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>身高,厘米为单位，如果是模特和主持人，则必填，否则为非必填项，此项由前段页面控制</t>
+    <t>艺人ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -727,147 +963,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>height</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skilled_style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_addr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(512)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mian_image_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>second_image_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(256)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>actorId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(32)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar（32）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kind</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>才艺风格，一级页面中每种风格的艺人只展示部分，点击更多查看全部。舞蹈分为街舞，流行舞，歌手分为摇滚，流行等，模特分为男模，女模；主持人分为男主持，女主持</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>displayed_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出演次数,参与过演出的次数，初始值按照艺人等级划分，公司将艺人分为高中低三个层级，初次录入资料的时候根据层级以及具体情况给定演出次数，以后每演出一次加一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visit_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>被查看次数，艺人被查看的次数，用户不需要登陆，只要点击了该艺人进入二级页面，查看次数+1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fans_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>粉丝数，爱心符号的标识，只有会员才可以点，点爱心标志，粉丝数+1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>加入时间，加入showmecoo公司的时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imageName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>形象照名，照片上传到服务器后的名字，存放形象照的目录固定，</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人等级评分，80－100的为高级，40-79的为中级，0-39的为低级，前期评分为主观评定，录入艺人的时候给打的分数，</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level_score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
+    <t>擅长的曲目风格，以逗号分割的字符串，eg：摇滚，流行，民俗</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -875,79 +971,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>display_price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_standard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>brief_introduction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(64)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>represantive_work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_standard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main_image_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>brief_introduction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level_score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>擅长的曲目风格，以逗号分割的字符串，eg：摇滚，流行，民俗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>歌手演员表－actor_singer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模特演员表－actor_model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别，男（1），女（2）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>模特的一级页面暂时按照男模和女模来区分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主持人演员表－actor_compere</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1138,7 +1162,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1187,6 +1211,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1264,7 +1290,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="79">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1300,6 +1326,7 @@
     <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1341,6 +1368,7 @@
     <cellStyle name="访问过的超链接" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1690,7 +1718,7 @@
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
+    <row r="1" spans="1:5" ht="23">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2050,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2034,7 +2062,7 @@
     <col min="9" max="9" width="158.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27">
+    <row r="1" spans="1:12" ht="25">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -2538,7 +2566,7 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2577,10 +2605,10 @@
         <v>130</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2588,13 +2616,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2602,13 +2630,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2616,13 +2644,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2630,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>125</v>
@@ -2644,13 +2672,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2658,13 +2686,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2672,13 +2700,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2686,13 +2714,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2700,13 +2728,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2714,13 +2742,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2728,13 +2756,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2759,10 +2787,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D76"/>
+  <dimension ref="A2:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2774,12 +2802,12 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -2804,13 +2832,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2818,13 +2846,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2832,13 +2860,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2846,13 +2874,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2860,13 +2888,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>229</v>
+        <v>173</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>228</v>
+        <v>92</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>227</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2874,13 +2902,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2888,13 +2916,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2902,13 +2930,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2916,13 +2944,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2930,13 +2958,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2944,13 +2972,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2958,185 +2986,185 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>167</v>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7">
+        <v>13</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
+      <c r="A20" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7">
-        <v>1</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>168</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="7">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>103</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="16" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -3161,13 +3189,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>131</v>
+        <v>217</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3175,13 +3203,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>166</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3189,13 +3217,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3203,13 +3231,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>217</v>
+        <v>92</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3217,13 +3245,13 @@
         <v>5</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>92</v>
+        <v>179</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3231,13 +3259,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>212</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3245,13 +3273,13 @@
         <v>7</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3259,13 +3287,13 @@
         <v>8</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3273,13 +3301,13 @@
         <v>9</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3287,119 +3315,119 @@
         <v>10</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="7">
-        <v>11</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>208</v>
-      </c>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="A50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>46</v>
+      <c r="A51" s="7">
+        <v>1</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>162</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>166</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>230</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3407,13 +3435,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3421,13 +3449,13 @@
         <v>8</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -3435,212 +3463,170 @@
         <v>9</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="7">
-        <v>10</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="7">
-        <v>11</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>208</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="18"/>
+      <c r="A65" s="7">
+        <v>1</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>46</v>
+      <c r="A66" s="7">
+        <v>3</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>232</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>217</v>
+        <v>91</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>92</v>
+        <v>179</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="7">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="7">
-        <v>9</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="7">
-        <v>10</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="7">
-        <v>11</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A63:D63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add work table design and update plan
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="开发计划时间安排" sheetId="1" r:id="rId1"/>
-    <sheet name="表结构设计-user" sheetId="2" r:id="rId2"/>
-    <sheet name="表结构设计－order" sheetId="3" r:id="rId3"/>
-    <sheet name="艺人表－actor" sheetId="4" r:id="rId4"/>
+    <sheet name="用户模块表结构" sheetId="2" r:id="rId2"/>
+    <sheet name="订单模块表结构" sheetId="3" r:id="rId3"/>
+    <sheet name="艺人模块表结构" sheetId="4" r:id="rId4"/>
+    <sheet name="作品模块表结构" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="262">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -551,10 +552,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>linkman_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>联系人姓名，默认是下单人的姓名，但是可以需改，不能为空</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -839,23 +836,167 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>varchar(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>represantive_work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>brief_introduction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(64)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>represantive_work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_standard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main_image_name</t>
+    <t>level_score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>歌手演员表－actor_singer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模特演员表－actor_model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主持人演员表－actor_compere</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar（45）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(45)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nick_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别，男（1），女（2）,必填字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人艺名，唯一字段，用于展示艺名以及区分重名艺人，必填字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人名字，必填字段t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>image_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擅长舞种，以逗号分割的字符串，eg 街舞，机械舞，爵士舞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人等级评分，80－100的为高级，40-79的为中级，0-39的为低级，前期评分为主观评定，录入艺人的时候给打的分数，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介，艺人自我简短介绍，不超过140个字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代表演出，以逗号分割的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺人ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出费用，不明确标出，作为以后的预留字段，如果为0则在页面写上“面议（总有惊喜）”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擅长的曲目风格，以逗号分割的字符串，eg：摇滚，流行，民俗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代表作品，唱的比较好的曲目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模特的一级页面暂时按照男模和女模来区分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主持人的一级页面暂时按照男模和女模来区分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>link_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推荐指数，0-100，不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片名称，不能为空，值为存于服务器上的图片名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作品简介，非必填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work_pictue_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visut_num</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -863,119 +1004,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>level_score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出地点，艺人接受的演出地点，以城市为单位，以逗号分割的字符串</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>歌手演员表－actor_singer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模特演员表－actor_model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主持人演员表－actor_compere</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar（45）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nick_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别，男（1），女（2）,必填字段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人艺名，唯一字段，用于展示艺名以及区分重名艺人，必填字段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人名字，必填字段t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>image_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人类型：舞者(1)，歌手(2)，模特(3)，主持人(4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>擅长舞种，以逗号分割的字符串，eg 街舞，机械舞，爵士舞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人等级评分，80－100的为高级，40-79的为中级，0-39的为低级，前期评分为主观评定，录入艺人的时候给打的分数，</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>简介，艺人自我简短介绍，不超过140个字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>副形象照名，在大图下方显示的小图，点击小图后在主图区域显示该图的大图，数据库中存放 以逗号分割的名字字符串，最多4个名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代表演出，以逗号分割的字符串</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>艺人ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出费用，不明确标出，作为以后的预留字段，如果为0则在页面写上“面议（总有惊喜）”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>擅长的曲目风格，以逗号分割的字符串，eg：摇滚，流行，民俗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代表作品，唱的比较好的曲目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模特的一级页面暂时按照男模和女模来区分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主持人的一级页面暂时按照男模和女模来区分</t>
+    <t>舞者图片作品－work_dancer_picture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作品ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作品名称，唯一字段，不能为空，不超过10个字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recommend_level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>picture_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看次数，非必填项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief_introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>舞者视频作品－work_dancer_video</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>video_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频名称，不能为空，值为存于服务器上的视频名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1162,7 +1255,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1211,6 +1304,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1290,7 +1391,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="87">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1327,6 +1428,10 @@
     <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1369,6 +1474,10 @@
     <cellStyle name="访问过的超链接" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2050,7 +2159,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2566,7 +2675,7 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2605,7 +2714,7 @@
         <v>130</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>131</v>
@@ -2616,13 +2725,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2630,13 +2739,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2644,13 +2753,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2658,7 +2767,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>125</v>
@@ -2672,13 +2781,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2686,13 +2795,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2700,13 +2809,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2714,13 +2823,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2728,13 +2837,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2742,13 +2851,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2756,13 +2865,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2789,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2802,12 +2911,12 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -2832,13 +2941,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2846,13 +2955,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2860,13 +2969,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>221</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2874,13 +2983,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2888,13 +2997,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2902,13 +3011,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2916,13 +3025,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>225</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2930,13 +3039,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2944,13 +3053,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2958,13 +3067,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2972,13 +3081,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2986,13 +3095,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3000,23 +3109,23 @@
         <v>13</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3041,13 +3150,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3055,13 +3164,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3069,13 +3178,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3083,13 +3192,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3097,13 +3206,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3111,13 +3220,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>103</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3125,13 +3234,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>179</v>
-      </c>
       <c r="D29" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3139,13 +3248,13 @@
         <v>8</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3153,18 +3262,18 @@
         <v>9</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>199</v>
-      </c>
       <c r="D31" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -3189,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3203,13 +3312,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3217,13 +3326,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3231,13 +3340,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3245,13 +3354,13 @@
         <v>5</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3259,13 +3368,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3273,13 +3382,13 @@
         <v>7</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3287,13 +3396,13 @@
         <v>8</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>179</v>
-      </c>
       <c r="D43" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3301,13 +3410,13 @@
         <v>9</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3315,18 +3424,18 @@
         <v>10</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -3351,13 +3460,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3365,13 +3474,13 @@
         <v>2</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -3379,13 +3488,13 @@
         <v>3</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3393,13 +3502,13 @@
         <v>4</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -3407,13 +3516,13 @@
         <v>5</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3421,13 +3530,13 @@
         <v>6</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3435,13 +3544,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>179</v>
-      </c>
       <c r="D57" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3449,13 +3558,13 @@
         <v>8</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -3463,18 +3572,18 @@
         <v>9</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -3499,13 +3608,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -3513,13 +3622,13 @@
         <v>3</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -3527,13 +3636,13 @@
         <v>4</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -3541,13 +3650,13 @@
         <v>5</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -3555,13 +3664,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -3569,13 +3678,13 @@
         <v>8</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -3583,13 +3692,13 @@
         <v>9</v>
       </c>
       <c r="B71" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>179</v>
-      </c>
       <c r="D71" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -3597,13 +3706,13 @@
         <v>10</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -3611,13 +3720,13 @@
         <v>11</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3642,4 +3751,331 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7">
+        <v>2</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7">
+        <v>3</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="7">
+        <v>4</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="7">
+        <v>5</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7">
+        <v>6</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="7">
+        <v>7</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="7">
+        <v>8</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7">
+        <v>9</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A15:D15"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add work module interface
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
+++ b/showmecoo-web-docs/src/main/resources/设计文档/概要设计/表结构设计.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="264">
   <si>
     <t>showmecoo产品开发计划时间安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -988,26 +988,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>work_pictue_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>varchar(20)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>visut_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>brief_introduction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>舞者图片作品－work_dancer_picture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>作品ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1052,10 +1040,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>舞者视频作品－work_dancer_video</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>video_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1069,6 +1053,30 @@
   </si>
   <si>
     <t>work_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频作品－work_video</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片作品－work_picture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visit_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>videoid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actorid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pictueid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1255,7 +1263,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1304,6 +1312,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1391,7 +1411,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="99">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1432,6 +1452,12 @@
     <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1478,6 +1504,12 @@
     <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3248,7 +3280,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>175</v>
@@ -3758,7 +3790,7 @@
   <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3766,11 +3798,14 @@
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -3795,13 +3830,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3809,7 +3844,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>91</v>
@@ -3823,13 +3858,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3837,7 +3872,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>92</v>
@@ -3851,7 +3886,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>91</v>
@@ -3865,13 +3900,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3879,13 +3914,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3893,13 +3928,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3907,7 +3942,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>178</v>
@@ -3918,7 +3953,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -3943,13 +3978,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3957,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>91</v>
@@ -3971,13 +4006,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3985,7 +4020,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>92</v>
@@ -3999,13 +4034,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4013,13 +4048,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4027,13 +4062,13 @@
         <v>7</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4041,13 +4076,13 @@
         <v>8</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4055,7 +4090,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>178</v>

</xml_diff>